<commit_message>
Added US localization without light sensor and created java doc
</commit_message>
<xml_diff>
--- a/Lab4_Localization/STAT_SHEET.xlsx
+++ b/Lab4_Localization/STAT_SHEET.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Trial #</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>STD  VAR</t>
+  </si>
+  <si>
+    <t>Rising-edge</t>
+  </si>
+  <si>
+    <t>Falling-Edge</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,28 +545,37 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B15" s="1">
         <f>AVERAGE(B3:B12)</f>
         <v>-5.8500000000000005</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C15" s="1">
         <f>AVERAGE(C3:C12)</f>
         <v>3.34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B16" s="1">
         <f>_xlfn.STDEV.S(B3:B12)</f>
         <v>1.8875321925142816</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C16" s="1">
         <f>_xlfn.STDEV.S(C3:C12)</f>
         <v>1.7411362828783841</v>
       </c>

</xml_diff>